<commit_message>
protect now looks for specified names only
</commit_message>
<xml_diff>
--- a/LP/Sheets.xlsx
+++ b/LP/Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\JuanCarlos\CL\LP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73FE0C5-5D19-473E-85BC-4C92431B66A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626F97E-FA5D-4A6F-A9AC-ADA26A122091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-4944" windowWidth="29016" windowHeight="15816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backend" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>Hojas Visibles</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Hojas Muy Ocultas</t>
   </si>
   <si>
-    <t>Hojas no protejidas</t>
-  </si>
-  <si>
     <t>Cuentas</t>
   </si>
   <si>
@@ -93,15 +90,9 @@
     <t>2 Ingresos BMV &amp; SIC</t>
   </si>
   <si>
-    <t>backend</t>
-  </si>
-  <si>
     <t>3 Ingresos 10% Ad - Dividendos</t>
   </si>
   <si>
-    <t>SheetNames</t>
-  </si>
-  <si>
     <t>Cap Gain Summary S-I</t>
   </si>
   <si>
@@ -271,6 +262,9 @@
   </si>
   <si>
     <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Hojas protejidas</t>
   </si>
 </sst>
 </file>
@@ -523,26 +517,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -551,10 +527,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
@@ -569,10 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
@@ -597,6 +565,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 3" xfId="2" xr:uid="{702E99B6-35D7-40B5-A072-707EEB127DFC}"/>
@@ -1280,7 +1274,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
@@ -1302,581 +1296,581 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.6">
       <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12" t="s">
+      <c r="S1" s="36"/>
+    </row>
+    <row r="2" spans="1:19" ht="19.8" thickBot="1">
+      <c r="A2" s="11">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>10</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15" t="s">
+    </row>
+    <row r="3" spans="1:19" ht="19.2">
+      <c r="B3" s="12"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="16"/>
-    </row>
-    <row r="2" spans="1:19" ht="19.8" thickBot="1">
-      <c r="A2" s="17">
-        <v>8</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
+      <c r="E3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="21">
+      <c r="N3" s="14"/>
+      <c r="P3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="14">
         <v>10</v>
       </c>
-      <c r="R2" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="24" t="s">
+      <c r="R3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="19.2">
-      <c r="B3" s="18"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26" t="s">
+    <row r="4" spans="1:19" ht="19.2">
+      <c r="B4" s="12"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M4" s="38"/>
+      <c r="N4" s="14"/>
+      <c r="P4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>10</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="P3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="21">
-        <v>10</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="24" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="19.2">
+      <c r="B5" s="12"/>
+      <c r="C5" s="21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="19.2">
-      <c r="B4" s="18"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="21"/>
-      <c r="P4" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>10</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="19.2">
-      <c r="B5" s="18"/>
-      <c r="C5" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22">
         <f t="shared" ref="M5:M17" si="0">SUM(D5:L5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="P5" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="21">
+      <c r="N5" s="14"/>
+      <c r="P5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="14">
         <v>10</v>
       </c>
-      <c r="R5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="24" t="s">
-        <v>47</v>
+      <c r="R5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="19.2">
-      <c r="B6" s="18"/>
-      <c r="C6" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30">
+      <c r="B6" s="12"/>
+      <c r="C6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="P6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="21">
+      <c r="N6" s="14"/>
+      <c r="P6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="14">
         <v>10</v>
       </c>
-      <c r="R6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" s="24" t="s">
-        <v>49</v>
+      <c r="R6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="19.2">
-      <c r="B7" s="18"/>
-      <c r="C7" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30">
+      <c r="B7" s="12"/>
+      <c r="C7" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="P7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q7" s="21">
+      <c r="N7" s="14"/>
+      <c r="P7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="14">
         <v>10</v>
       </c>
-      <c r="R7" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="24" t="s">
-        <v>51</v>
+      <c r="R7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="19.2">
-      <c r="B8" s="18"/>
-      <c r="C8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30">
+      <c r="B8" s="12"/>
+      <c r="C8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N8" s="21"/>
-      <c r="P8" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" s="21">
+      <c r="N8" s="14"/>
+      <c r="P8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="14">
         <v>10</v>
       </c>
-      <c r="R8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="S8" s="24" t="s">
-        <v>53</v>
+      <c r="R8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="19.2">
-      <c r="B9" s="18"/>
-      <c r="C9" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30">
+      <c r="B9" s="12"/>
+      <c r="C9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="P9" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="21">
+      <c r="N9" s="14"/>
+      <c r="P9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="14">
         <v>10</v>
       </c>
-      <c r="R9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" s="24" t="s">
-        <v>55</v>
+      <c r="R9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="19.2">
-      <c r="B10" s="18"/>
-      <c r="C10" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30">
+      <c r="B10" s="12"/>
+      <c r="C10" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N10" s="21"/>
-      <c r="P10" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q10" s="21">
+      <c r="N10" s="14"/>
+      <c r="P10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="14">
         <v>10</v>
       </c>
-      <c r="R10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="S10" s="24" t="s">
-        <v>57</v>
+      <c r="R10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="19.2">
-      <c r="B11" s="18"/>
-      <c r="C11" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30">
+      <c r="B11" s="12"/>
+      <c r="C11" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N11" s="21"/>
-      <c r="P11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q11" s="21">
+      <c r="N11" s="14"/>
+      <c r="P11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="14">
         <v>9</v>
       </c>
-      <c r="R11" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="S11" s="31" t="s">
-        <v>59</v>
+      <c r="R11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="19.2">
-      <c r="B12" s="18"/>
-      <c r="C12" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30">
+      <c r="B12" s="12"/>
+      <c r="C12" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="21"/>
-      <c r="P12" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q12" s="21">
+      <c r="N12" s="14"/>
+      <c r="P12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="14">
         <v>9</v>
       </c>
-      <c r="R12" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="S12" s="31" t="s">
-        <v>61</v>
+      <c r="R12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="19.2">
-      <c r="B13" s="18"/>
-      <c r="C13" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30">
+      <c r="B13" s="12"/>
+      <c r="C13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="21"/>
-      <c r="P13" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="21">
+      <c r="N13" s="14"/>
+      <c r="P13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="14">
         <v>9</v>
       </c>
-      <c r="R13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>63</v>
+      <c r="R13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="19.8" thickBot="1">
-      <c r="B14" s="18"/>
-      <c r="C14" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30">
+      <c r="B14" s="12"/>
+      <c r="C14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="21"/>
-      <c r="P14" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14" s="33">
+      <c r="N14" s="14"/>
+      <c r="P14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="25">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="19.2">
-      <c r="B15" s="18"/>
-      <c r="C15" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30">
+      <c r="B15" s="12"/>
+      <c r="C15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="21"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="19.2">
-      <c r="B16" s="18"/>
-      <c r="C16" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30">
+      <c r="B16" s="12"/>
+      <c r="C16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N16" s="21"/>
+      <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" ht="19.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30">
+      <c r="B17" s="12"/>
+      <c r="C17" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N17" s="21"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" ht="19.2">
-      <c r="B18" s="18"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="35">
+      <c r="B18" s="12"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="27">
         <f>SUM(M6:M17)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="21"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="2:14" ht="19.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="N19" s="21"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="N19" s="14"/>
     </row>
     <row r="20" spans="2:14" ht="19.8" thickBot="1">
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="33"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="25"/>
     </row>
     <row r="21" spans="2:14" ht="19.2">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1895,8 +1889,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5546875" defaultRowHeight="15"/>
@@ -1917,169 +1911,231 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="C8lpWMiq3GnERrtK9j83cZQ0WQBgDSz9PNqikuXGTIjK4F8K9tvYQeyzT077j2pMYLYM1LOmkJFIFRr01N5P8A==" saltValue="uCYEDRDuBL26cf0UwuzKkA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed columns and sheets protection
</commit_message>
<xml_diff>
--- a/LP/Sheets.xlsx
+++ b/LP/Sheets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\JuanCarlos\CL\LP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626F97E-FA5D-4A6F-A9AC-ADA26A122091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC04D92-218A-4076-8175-533F6D777705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>Hojas Visibles</t>
   </si>
@@ -611,7 +611,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cuentas"/>
@@ -811,7 +811,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="SheetNames"/>
@@ -1889,8 +1889,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5546875" defaultRowHeight="15"/>
@@ -1946,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1954,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1962,7 +1962,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1970,7 +1970,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1978,7 +1978,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1986,15 +1986,15 @@
         <v>11</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2002,7 +2002,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2010,7 +2010,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2018,7 +2018,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2026,15 +2026,15 @@
         <v>16</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>19</v>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2042,7 +2042,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2050,7 +2050,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2058,7 +2058,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2066,7 +2066,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2074,7 +2074,7 @@
         <v>22</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2082,47 +2082,32 @@
         <v>23</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5">

</xml_diff>